<commit_message>
gitkeep files, run.py outside of methods folder
</commit_message>
<xml_diff>
--- a/data/Inputs/excel/Demand_dependancy.xlsx
+++ b/data/Inputs/excel/Demand_dependancy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessio\programming_practise\VISSIM_work\VISSIM\data\inputs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7B9679-235E-4D32-8CB8-C2F1E0B2D15F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1866A9A2-513B-4154-9900-15DE54F18269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:BH80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2233,7 +2233,7 @@
       <formula>-0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D16" xr:uid="{7697CC59-4FFB-4E32-BDCA-87774B32985C}">
       <formula1>"Pedestrian, Traffic, Traffic &amp; Ped"</formula1>
     </dataValidation>
@@ -2248,9 +2248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
abstracted the filename process to a fucntion. Commented and refactored
</commit_message>
<xml_diff>
--- a/data/Inputs/excel/Demand_dependancy.xlsx
+++ b/data/Inputs/excel/Demand_dependancy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessio\programming_practise\VISSIM_work\VISSIM\data\inputs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1866A9A2-513B-4154-9900-15DE54F18269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05874C47-6B07-4D2F-9814-D2B8D9019088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:BH80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="5" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="21">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" s="32">
         <v>2</v>
@@ -1183,7 +1183,7 @@
       </c>
       <c r="G5" s="2" t="str">
         <f t="shared" ref="G5:G16" si="0">A5&amp;"_"&amp;E5&amp;"_"&amp;"green"</f>
-        <v>23_2_green</v>
+        <v>20_2_green</v>
       </c>
       <c r="H5" s="38">
         <v>48</v>

</xml_diff>